<commit_message>
Updating Extruder Steps per mm
</commit_message>
<xml_diff>
--- a/Stepper Motors.xlsx
+++ b/Stepper Motors.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="2055" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <definedName name="InitialHeight">'[1]Measured Offsets'!$B$1</definedName>
     <definedName name="ProbeLength">'[1]Find Delta Radius'!$B$1</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Motor</t>
   </si>
@@ -122,18 +122,34 @@
   </si>
   <si>
     <t>Step Angle</t>
+  </si>
+  <si>
+    <t>Extruder Adjustment</t>
+  </si>
+  <si>
+    <t>Expected Extruded Length</t>
+  </si>
+  <si>
+    <t>Actual Extruded Length</t>
+  </si>
+  <si>
+    <t>Corrected Steps per mm</t>
+  </si>
+  <si>
+    <t>Attempt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +171,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -164,7 +188,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -181,14 +205,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
@@ -202,13 +251,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Heading 1" xfId="4" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="3"/>
@@ -615,31 +677,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.19921875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.53125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="12.19921875" style="1"/>
+    <col min="1" max="1" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -658,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -685,7 +751,7 @@
         <v>552.5333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -710,14 +776,77 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I5" s="1">
         <f>100/120</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <f>I5*H2</f>
         <v>460.44444444444446</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="14">
+        <v>1</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="15">
+        <f>H2</f>
+        <v>552.5333333333333</v>
+      </c>
+      <c r="C13" s="15">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="16">
+        <v>100</v>
+      </c>
+      <c r="C14" s="16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="16">
+        <v>120</v>
+      </c>
+      <c r="C15" s="16">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="18">
+        <f>B13/B15*B14</f>
+        <v>460.4444444444444</v>
+      </c>
+      <c r="C16" s="18">
+        <f>C13/C15*C14</f>
+        <v>446.60194174757282</v>
       </c>
     </row>
   </sheetData>
@@ -737,17 +866,17 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -755,7 +884,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -766,7 +895,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -777,7 +906,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -790,7 +919,7 @@
         <v>5.18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -801,7 +930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>25</v>
       </c>
@@ -814,7 +943,7 @@
         <v>659.53808417281425</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -822,7 +951,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -830,7 +959,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -839,7 +968,7 @@
         <v>0.68493150684931503</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -861,26 +990,26 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="4"/>
-    <col min="3" max="4" width="12.46484375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C2" s="11" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -903,7 +1032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -930,7 +1059,7 @@
         <v>60.000000000000014</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
@@ -957,7 +1086,7 @@
         <v>60.000000000000057</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>

</xml_diff>